<commit_message>
charts page is added
</commit_message>
<xml_diff>
--- a/Requirement/Pending Items.xlsx
+++ b/Requirement/Pending Items.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Functionality Part</t>
   </si>
@@ -64,6 +64,21 @@
   </si>
   <si>
     <t>Ownership</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Half Done</t>
+  </si>
+  <si>
+    <t>Almost Done</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
+    <t>Hold - Admin Page</t>
   </si>
 </sst>
 </file>
@@ -442,6 +457,9 @@
       <c r="B3" t="s">
         <v>4</v>
       </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4">
@@ -450,6 +468,9 @@
       <c r="B4" t="s">
         <v>5</v>
       </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5">
@@ -458,6 +479,9 @@
       <c r="B5" t="s">
         <v>9</v>
       </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="6" spans="1:10">
       <c r="A6">
@@ -466,6 +490,9 @@
       <c r="B6" t="s">
         <v>6</v>
       </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="7" spans="1:10">
       <c r="A7">
@@ -474,6 +501,9 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
       <c r="A8">
@@ -482,6 +512,9 @@
       <c r="B8" t="s">
         <v>8</v>
       </c>
+      <c r="C8" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="9" spans="1:10">
       <c r="A9">
@@ -490,6 +523,9 @@
       <c r="B9" t="s">
         <v>10</v>
       </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:10">
       <c r="A10">
@@ -498,6 +534,9 @@
       <c r="B10" t="s">
         <v>11</v>
       </c>
+      <c r="C10" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:10">
       <c r="A11">
@@ -505,6 +544,9 @@
       </c>
       <c r="B11" t="s">
         <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:10">

</xml_diff>